<commit_message>
1. fix history trend bug. 2. fix signal logging behavior
</commit_message>
<xml_diff>
--- a/report_template/chart_export.xlsx
+++ b/report_template/chart_export.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\webApp\AQM\report_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\webApp\Datalogger2\report_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DCB74A-3B30-4CF2-8E05-B5348A7304EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
@@ -353,16 +354,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="14.625" style="1"/>
+    <col min="1" max="16384" width="20" style="1"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>